<commit_message>
Update Master dan lainnya
</commit_message>
<xml_diff>
--- a/storage/app/public/template_material.xlsx
+++ b/storage/app/public/template_material.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t xml:space="preserve">material</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">deskripsi</t>
   </si>
   <si>
-    <t xml:space="preserve">mrp</t>
-  </si>
-  <si>
     <t xml:space="preserve">mtyp</t>
   </si>
   <si>
@@ -38,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">bun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valcl</t>
   </si>
   <si>
     <t xml:space="preserve">102KM34-CXXX-BK74</t>
@@ -79,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,22 +155,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -194,80 +187,56 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="n">
+        <v>10406</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1320</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>10406</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>7900</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1320</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>10406</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>7900</v>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1320</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>10406</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>7900</v>
+      <c r="E4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>